<commit_message>
Update Design Input File_Robert_Umali_V25-01.xlsx
</commit_message>
<xml_diff>
--- a/Design Input Files/Design Input File_Robert_Umali_V25-01.xlsx
+++ b/Design Input Files/Design Input File_Robert_Umali_V25-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocke\OneDrive\Documents\GitHub\Aero-Design-Lab\Design Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roum9599\Documents\GitHub\Aero-Design-Lab\Design Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2B5F82-0E05-418C-A6CC-754CE40B80E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE999F8A-E788-4F4D-8B7D-D6453711B59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1470" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{904FC4B5-3CDE-421B-8E98-23A2C72E8C1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{904FC4B5-3CDE-421B-8E98-23A2C72E8C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable Reference" sheetId="12" r:id="rId1"/>
@@ -44,6 +44,9 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1184,7 +1187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="226">
   <si>
     <t>Length_f</t>
   </si>
@@ -1859,6 +1862,9 @@
   </si>
   <si>
     <t>NACA 0011</t>
+  </si>
+  <si>
+    <t>DLG</t>
   </si>
 </sst>
 </file>
@@ -2855,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14EA422-282A-4DE2-BD24-B68BB0CEE4E3}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4013,15 +4019,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADD393-55AB-49FB-9382-D2896E9EB980}">
   <dimension ref="A1:AR21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:AR22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="7" customWidth="1"/>
-    <col min="3" max="11" width="8.85546875" style="7"/>
+    <col min="3" max="7" width="8.85546875" style="7"/>
+    <col min="8" max="8" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.85546875" style="7"/>
     <col min="12" max="12" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.85546875" style="7" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" style="7"/>
@@ -4183,7 +4191,7 @@
         <v>1600</v>
       </c>
       <c r="C3" s="7">
-        <v>10.5</v>
+        <v>15</v>
       </c>
       <c r="D3" s="7">
         <v>0.7</v>
@@ -4307,6 +4315,20 @@
       </c>
       <c r="AR3" s="7" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1600</v>
+      </c>
+      <c r="C4" s="7">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.7</v>
       </c>
     </row>
     <row r="21" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4688,8 +4710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51281E0C-C3D7-4E6E-9445-AF10F5AA801D}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4774,7 +4796,7 @@
         <v>223</v>
       </c>
       <c r="B3" s="7">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="C3" s="7">
         <v>0.05</v>
@@ -4822,7 +4844,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="7">
-        <v>0.16</v>
+        <v>160</v>
       </c>
       <c r="S3" s="7">
         <v>0.33</v>

</xml_diff>

<commit_message>
fixed sheet. messed up code
</commit_message>
<xml_diff>
--- a/Design Input Files/Design Input File_Robert_Umali_V25-01.xlsx
+++ b/Design Input Files/Design Input File_Robert_Umali_V25-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocke\OneDrive\Documents\GitHub\Aero-Design-Lab\Design Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2B5F82-0E05-418C-A6CC-754CE40B80E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47604070-9BF0-42D6-B9AC-1DB138B5CB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1470" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{904FC4B5-3CDE-421B-8E98-23A2C72E8C1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{904FC4B5-3CDE-421B-8E98-23A2C72E8C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable Reference" sheetId="12" r:id="rId1"/>
@@ -1184,7 +1184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="226">
   <si>
     <t>Length_f</t>
   </si>
@@ -1855,10 +1855,13 @@
     <t>NACA 0010</t>
   </si>
   <si>
-    <t>HighAR</t>
-  </si>
-  <si>
     <t>NACA 0011</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>HighAR5</t>
   </si>
 </sst>
 </file>
@@ -2196,13 +2199,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2853,10 +2856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14EA422-282A-4DE2-BD24-B68BB0CEE4E3}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2871,7 @@
     <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>160</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>204</v>
       </c>
@@ -2896,8 +2899,11 @@
       <c r="D2" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>204</v>
       </c>
@@ -2910,8 +2916,11 @@
       <c r="D3" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>204</v>
       </c>
@@ -2924,8 +2933,11 @@
       <c r="D4" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>204</v>
       </c>
@@ -2938,8 +2950,11 @@
       <c r="D5" s="8" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>204</v>
       </c>
@@ -2952,8 +2967,11 @@
       <c r="D6" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>204</v>
       </c>
@@ -2966,8 +2984,11 @@
       <c r="D7" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>204</v>
       </c>
@@ -2980,8 +3001,11 @@
       <c r="D8" s="8" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>204</v>
       </c>
@@ -2994,8 +3018,11 @@
       <c r="D9" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>204</v>
       </c>
@@ -3008,8 +3035,11 @@
       <c r="D10" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>204</v>
       </c>
@@ -3022,8 +3052,11 @@
       <c r="D11" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>204</v>
       </c>
@@ -3036,8 +3069,11 @@
       <c r="D12" s="8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>204</v>
       </c>
@@ -3050,8 +3086,11 @@
       <c r="D13" s="8" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>204</v>
       </c>
@@ -3064,8 +3103,11 @@
       <c r="D14" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>204</v>
       </c>
@@ -3078,8 +3120,11 @@
       <c r="D15" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>204</v>
       </c>
@@ -3092,8 +3137,11 @@
       <c r="D16" s="8" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>204</v>
       </c>
@@ -3106,8 +3154,11 @@
       <c r="D17" s="8" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>204</v>
       </c>
@@ -3120,8 +3171,11 @@
       <c r="D18" s="8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>204</v>
       </c>
@@ -3134,8 +3188,11 @@
       <c r="D19" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>204</v>
       </c>
@@ -3148,8 +3205,11 @@
       <c r="D20" s="8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>204</v>
       </c>
@@ -3162,8 +3222,11 @@
       <c r="D21" s="8" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>204</v>
       </c>
@@ -3176,8 +3239,11 @@
       <c r="D22" s="8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>204</v>
       </c>
@@ -3190,8 +3256,11 @@
       <c r="D23" s="8" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>204</v>
       </c>
@@ -3204,8 +3273,11 @@
       <c r="D24" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>204</v>
       </c>
@@ -3218,8 +3290,11 @@
       <c r="D25" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>204</v>
       </c>
@@ -3232,8 +3307,11 @@
       <c r="D26" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>204</v>
       </c>
@@ -3246,8 +3324,11 @@
       <c r="D27" s="8" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>204</v>
       </c>
@@ -3260,8 +3341,11 @@
       <c r="D28" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>204</v>
       </c>
@@ -3274,8 +3358,11 @@
       <c r="D29" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>204</v>
       </c>
@@ -3288,8 +3375,11 @@
       <c r="D30" s="8" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>204</v>
       </c>
@@ -3302,8 +3392,11 @@
       <c r="D31" s="8" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>204</v>
       </c>
@@ -3316,8 +3409,11 @@
       <c r="D32" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>204</v>
       </c>
@@ -3330,8 +3426,11 @@
       <c r="D33" s="8" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>204</v>
       </c>
@@ -3344,8 +3443,11 @@
       <c r="D34" s="8" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>204</v>
       </c>
@@ -3358,8 +3460,11 @@
       <c r="D35" s="8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>204</v>
       </c>
@@ -3372,8 +3477,11 @@
       <c r="D36" s="8" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>204</v>
       </c>
@@ -3386,8 +3494,11 @@
       <c r="D37" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>204</v>
       </c>
@@ -3401,7 +3512,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>204</v>
       </c>
@@ -3415,7 +3526,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>204</v>
       </c>
@@ -3429,7 +3540,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>204</v>
       </c>
@@ -3443,7 +3554,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>204</v>
       </c>
@@ -3457,7 +3568,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>204</v>
       </c>
@@ -3471,7 +3582,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>204</v>
       </c>
@@ -3485,7 +3596,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>204</v>
       </c>
@@ -3499,7 +3610,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>161</v>
       </c>
@@ -3513,7 +3624,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>161</v>
       </c>
@@ -3527,7 +3638,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>161</v>
       </c>
@@ -4011,17 +4122,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADD393-55AB-49FB-9382-D2896E9EB980}">
-  <dimension ref="A1:AR21"/>
+  <dimension ref="A1:AR20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:AR22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="7" customWidth="1"/>
-    <col min="3" max="11" width="8.85546875" style="7"/>
+    <col min="3" max="7" width="8.85546875" style="7"/>
+    <col min="8" max="8" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="7"/>
     <col min="12" max="12" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.85546875" style="7" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" style="7"/>
@@ -4175,144 +4289,147 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" s="7">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="7">
         <v>1600</v>
       </c>
-      <c r="C3" s="7">
-        <v>10.5</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C2" s="7">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7">
         <v>0.7</v>
       </c>
-      <c r="E3" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="F3" s="7">
-        <v>8.75</v>
-      </c>
-      <c r="G3" s="7">
-        <v>2E-3</v>
-      </c>
-      <c r="H3" s="7">
-        <v>5.0299999999999997E-3</v>
-      </c>
-      <c r="I3" s="7">
-        <v>5.0299999999999997E-3</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="K3" s="7">
-        <v>1.18</v>
-      </c>
-      <c r="L3" s="7" t="s">
+      <c r="E2" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="F2" s="7">
+        <f>D2/E2</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1.5874999999999999E-3</v>
+      </c>
+      <c r="H2" s="7">
+        <f>PI()*(E2/2)^2</f>
+        <v>2.8274333882308137E-3</v>
+      </c>
+      <c r="I2" s="7">
+        <f>PI()*(0.011/2)^2</f>
+        <v>9.5033177771091233E-5</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K2" s="7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0.122</v>
+      </c>
+      <c r="O2" s="7">
+        <v>16</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>5</v>
+      </c>
+      <c r="R2" s="7">
+        <v>0</v>
+      </c>
+      <c r="S2" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="U2" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V2" s="7">
+        <v>3.1E-2</v>
+      </c>
+      <c r="W2" s="7">
+        <v>5</v>
+      </c>
+      <c r="X2" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>0.1115</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AB2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M3" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="O3" s="7">
-        <v>12.5</v>
-      </c>
-      <c r="P3" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="Q3" s="7">
+      <c r="AC2" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AG2" s="7">
+        <v>25</v>
+      </c>
+      <c r="AH2" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="AI2" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK2" s="7">
         <v>0</v>
       </c>
-      <c r="R3" s="7">
+      <c r="AL2" s="7">
         <v>0</v>
       </c>
-      <c r="S3" s="7">
-        <v>1.06</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="U3" s="7">
-        <v>1.6E-2</v>
-      </c>
-      <c r="V3" s="7">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="W3" s="7">
-        <v>5</v>
-      </c>
-      <c r="X3" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="Y3" s="7">
+      <c r="AM2" s="7">
         <v>0</v>
       </c>
-      <c r="Z3" s="7">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="AA3" s="7">
-        <v>1.08</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC3" s="7">
+      <c r="AN2" s="7">
         <v>0</v>
       </c>
-      <c r="AD3" s="7">
+      <c r="AO2" s="7">
         <v>0</v>
       </c>
-      <c r="AE3" s="7">
+      <c r="AP2" s="7">
         <v>0</v>
       </c>
-      <c r="AF3" s="7">
+      <c r="AQ2" s="7">
         <v>0</v>
       </c>
-      <c r="AG3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
+      <c r="AR2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="AK3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="7">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="20" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB21 AB23:AB51 L3:L21 L23:L51 T3:T21 T23:T51 AR3:AR21 AR23:AR51 AJ3:AJ21 AJ23:AJ51" xr:uid="{F18DD44F-5AC9-42F9-970E-83AFBD39DB9D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB22:AB50 L22:L50 T22:T50 AR22:AR50 AJ22:AJ50 AB2:AB20 AJ2:AJ20 AR2:AR20 T2:T20 L2:L20" xr:uid="{F18DD44F-5AC9-42F9-970E-83AFBD39DB9D}">
       <formula1>MATERIALS</formula1>
     </dataValidation>
   </dataValidations>
@@ -4323,10 +4440,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538960B4-04F0-4DA1-BF31-3569558CC234}">
-  <dimension ref="A1:AY21"/>
+  <dimension ref="A1:AY20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AY7" sqref="AY7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4501,183 +4618,163 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="str">
-        <f>Main_Input!A3</f>
-        <v>HighAR</v>
-      </c>
-      <c r="B3" s="18" t="s">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="str">
+        <f>Main_Input!A2</f>
+        <v>HighAR5</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C2" s="18">
         <v>0.12</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D2" s="18">
         <v>0.3</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E2" s="18">
         <v>-0.28499999999999998</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F2" s="18">
         <v>-0.19</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G2" s="18">
         <v>-9.5000000000000001E-2</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H2" s="18">
         <v>0</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I2" s="18">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J2" s="18">
         <v>0.19</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K2" s="18">
         <v>0.28499999999999998</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L2" s="18">
         <v>0.38</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M2" s="18">
         <v>0.47499999999999998</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N2" s="18">
         <v>0.56999999999999995</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O2" s="18">
         <v>0.66500000000000004</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P2" s="18">
         <v>0.76</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q2" s="18">
         <v>0.85499999999999998</v>
       </c>
-      <c r="R3" s="18">
+      <c r="R2" s="18">
         <v>0.95</v>
       </c>
-      <c r="S3" s="18">
+      <c r="S2" s="18">
         <v>1.0449999999999999</v>
       </c>
-      <c r="T3" s="18">
+      <c r="T2" s="18">
         <v>1.1399999999999999</v>
       </c>
-      <c r="U3" s="18">
+      <c r="U2" s="18">
         <v>1.1499999999999999</v>
       </c>
-      <c r="V3" s="18">
+      <c r="V2" s="18">
         <v>1.05</v>
       </c>
-      <c r="W3" s="18">
+      <c r="W2" s="18">
         <v>1.1499999999999999</v>
       </c>
-      <c r="X3" s="19">
+      <c r="X2" s="19">
         <v>3.8109999999999998E-2</v>
       </c>
-      <c r="Y3" s="19">
+      <c r="Y2" s="19">
         <v>3.313E-2</v>
       </c>
-      <c r="Z3" s="19">
+      <c r="Z2" s="19">
         <v>2.9219999999999999E-2</v>
       </c>
-      <c r="AA3" s="19">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="AB3" s="19">
+      <c r="AA2" s="19">
+        <v>2.64E-2</v>
+      </c>
+      <c r="AB2" s="19">
         <v>2.4660000000000001E-2</v>
       </c>
-      <c r="AC3" s="19">
+      <c r="AC2" s="19">
         <v>2.401E-2</v>
       </c>
-      <c r="AD3" s="19">
+      <c r="AD2" s="19">
         <v>2.443E-2</v>
       </c>
-      <c r="AE3" s="19">
+      <c r="AE2" s="19">
         <v>2.5940000000000001E-2</v>
       </c>
-      <c r="AF3" s="19">
+      <c r="AF2" s="19">
         <v>2.8539999999999999E-2</v>
       </c>
-      <c r="AG3" s="19">
+      <c r="AG2" s="19">
         <v>3.2210000000000003E-2</v>
       </c>
-      <c r="AH3" s="19">
+      <c r="AH2" s="19">
         <v>3.6970000000000003E-2</v>
       </c>
-      <c r="AI3" s="19">
+      <c r="AI2" s="19">
         <v>4.2819999999999997E-2</v>
       </c>
-      <c r="AJ3" s="19">
+      <c r="AJ2" s="19">
         <v>4.9739999999999999E-2</v>
       </c>
-      <c r="AK3" s="19">
+      <c r="AK2" s="19">
         <v>5.7750000000000003E-2</v>
       </c>
-      <c r="AL3" s="19">
+      <c r="AL2" s="19">
         <v>6.6839999999999997E-2</v>
       </c>
-      <c r="AM3" s="19">
+      <c r="AM2" s="19">
         <v>7.7020000000000005E-2</v>
       </c>
-      <c r="AN3" s="19">
+      <c r="AN2" s="19">
         <v>9.8150000000000001E-2</v>
       </c>
-      <c r="AO3" s="19">
+      <c r="AO2" s="19">
         <v>0.10735</v>
       </c>
-      <c r="AP3" s="18">
+      <c r="AP2" s="18">
         <v>2.4E-2</v>
       </c>
-      <c r="AQ3" s="18" t="s">
+      <c r="AQ2" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="AR3" s="18">
+      <c r="AR2" s="18">
         <v>0.09</v>
       </c>
-      <c r="AS3" s="18">
+      <c r="AS2" s="18">
         <v>0.3</v>
       </c>
-      <c r="AT3" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="AU3" s="18">
+      <c r="AT2" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="AU2" s="18">
         <v>0.1</v>
       </c>
-      <c r="AV3" s="18">
+      <c r="AV2" s="18">
         <v>0.3</v>
       </c>
-      <c r="AW3" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="AX3" s="18">
+      <c r="AW2" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX2" s="18">
         <v>0.1</v>
       </c>
-      <c r="AY3" s="18">
+      <c r="AY2" s="18">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="19"/>
-      <c r="AI4" s="19"/>
-      <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-      <c r="AL4" s="19"/>
-      <c r="AM4" s="19"/>
-      <c r="AN4" s="19"/>
-      <c r="AO4" s="19"/>
-    </row>
-    <row r="21" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4686,10 +4783,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51281E0C-C3D7-4E6E-9445-AF10F5AA801D}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4769,70 +4866,94 @@
         <v>182</v>
       </c>
     </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="str">
+        <f>Main_Input!A2</f>
+        <v>HighAR5</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="I2" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.62</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="O2" s="7">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>0</v>
+      </c>
+      <c r="R2" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="S2" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="T2" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U2" s="7">
+        <v>0.09</v>
+      </c>
+    </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.09</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.17</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="I3" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0.62</v>
-      </c>
-      <c r="K3" s="7">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="L3" s="7">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0</v>
-      </c>
-      <c r="P3" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>0</v>
-      </c>
-      <c r="R3" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="S3" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="T3" s="7">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="U3" s="7">
-        <v>0.09</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -5202,30 +5323,7 @@
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-    </row>
-    <row r="21" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:21" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5238,7 +5336,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5570,7 +5668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB49278-C885-4626-918F-22B9EA08CAD8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>

</xml_diff>